<commit_message>
Modify ipynb files relate to Figure3
</commit_message>
<xml_diff>
--- a/raw_data/cat_deletion/deletion_fraction/YK0083/3hr/190413.xlsx
+++ b/raw_data/cat_deletion/deletion_fraction/YK0083/3hr/190413.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuta_koganezawa/Documents/Wakamoto_lab/paper_data/raw_data/cat_deletion/deletion_fraction/YK0083/3hr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuta_koganezawa/Documents/Wakamoto_lab/paper_data/Phenotypic_Buffering/raw_data/cat_deletion/deletion_fraction/YK0083/3hr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1043CB-F983-1647-902B-5DE1FA9DEEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64175500-6140-3B42-9CB4-663E7AF20697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1600" windowWidth="25000" windowHeight="15000" activeTab="2" xr2:uid="{7F690851-09F0-A84B-9670-77FE62F3FAA4}"/>
+    <workbookView xWindow="2760" yWindow="1600" windowWidth="25000" windowHeight="15000" xr2:uid="{7F690851-09F0-A84B-9670-77FE62F3FAA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Probability" sheetId="1" r:id="rId1"/>
@@ -334,9 +334,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -348,8 +357,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -668,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6713B7EC-9982-9F4B-9EBF-523AC103F1D8}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="20"/>
@@ -1434,7 +1446,7 @@
   <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="20"/>
@@ -2060,7 +2072,7 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>12</v>
       </c>
       <c r="B19">
@@ -3710,7 +3722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98725AF-FF54-B64C-BC0A-2A7C894A13FA}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:C70"/>
     </sheetView>
   </sheetViews>

</xml_diff>